<commit_message>
mejora en los tracker de fechas de vencimiento
</commit_message>
<xml_diff>
--- a/Documents/ejemplo.xlsx
+++ b/Documents/ejemplo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medtronic-my.sharepoint.com/personal/rodrij545_medtronic_com/Documents/Desktop/Tracker/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8B2B00B-5025-4ED6-966E-9F3DD0DEFE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D8B2B00B-5025-4ED6-966E-9F3DD0DEFE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D25AD6BA-7459-48F4-9928-30E9E608AA38}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{992961B0-246D-47A7-B660-DC62D0D50147}"/>
+    <workbookView minimized="1" xWindow="-19110" yWindow="6795" windowWidth="14400" windowHeight="7365" xr2:uid="{992961B0-246D-47A7-B660-DC62D0D50147}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -490,10 +490,13 @@
   <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A34"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>